<commit_message>
added by tesa for condition login binding Bank 2
</commit_message>
<xml_diff>
--- a/Data Files/Bank 2/bank2.xlsx
+++ b/Data Files/Bank 2/bank2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>email</t>
   </si>
@@ -33,6 +33,12 @@
     <t>password</t>
   </si>
   <si>
+    <t>email2</t>
+  </si>
+  <si>
+    <t>password2</t>
+  </si>
+  <si>
     <t>rezamuhammadsaput@gmail.com</t>
   </si>
   <si>
@@ -47,10 +53,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -70,23 +76,56 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -98,9 +137,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -108,15 +160,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -124,14 +175,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -139,30 +183,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -176,44 +204,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -228,13 +234,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -246,55 +372,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -306,109 +414,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -437,11 +449,59 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -463,50 +523,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
       <bottom style="double">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -525,174 +546,174 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1024,20 +1045,20 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="4" width="19.4444444444444" style="3" customWidth="1"/>
+    <col min="1" max="4" width="19.4444444444444" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1050,37 +1071,52 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="29.7777777777778" customWidth="1"/>
-    <col min="2" max="3" width="14.2222222222222" customWidth="1"/>
+    <col min="2" max="2" width="14.2222222222222" customWidth="1"/>
+    <col min="3" max="3" width="39.5555555555556" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
+    <row r="2" spans="1:4">
+      <c r="A2" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="rezamuhammadsaput@gmail.com"/>
+    <hyperlink ref="C2" r:id="rId1" display="rezamuhammadsaput@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -1103,7 +1139,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added by tesa for regis and login
</commit_message>
<xml_diff>
--- a/Data Files/Bank 2/bank2.xlsx
+++ b/Data Files/Bank 2/bank2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9335" activeTab="1"/>
+    <workbookView windowWidth="23040" windowHeight="9335"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>email</t>
   </si>
@@ -28,6 +28,15 @@
   </si>
   <si>
     <t>confirmpass</t>
+  </si>
+  <si>
+    <t>rattesa.ponto@work.briagro.c.id</t>
+  </si>
+  <si>
+    <t>tesa</t>
+  </si>
+  <si>
+    <t>123456Amberegul</t>
   </si>
   <si>
     <t>password</t>
@@ -53,9 +62,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
@@ -75,6 +84,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -82,8 +114,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -97,27 +130,49 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -129,16 +184,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -146,51 +194,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -204,16 +207,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -240,13 +249,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -258,7 +393,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -270,37 +417,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -312,115 +429,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -445,6 +454,65 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -482,67 +550,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -551,148 +560,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -715,7 +724,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1037,32 +1046,50 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="4" width="19.4444444444444" style="6" customWidth="1"/>
+    <col min="1" max="1" width="32.3333333333333" style="5" customWidth="1"/>
+    <col min="2" max="4" width="19.4444444444444" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="rattesa.ponto@work.briagro.c.id"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
@@ -1073,7 +1100,7 @@
   <sheetPr/>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -1090,27 +1117,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1139,7 +1166,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added by tesa tc_transfer bank2
</commit_message>
<xml_diff>
--- a/Data Files/Bank 2/bank2.xlsx
+++ b/Data Files/Bank 2/bank2.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9335"/>
+    <workbookView windowWidth="23040" windowHeight="9335" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="1" r:id="rId1"/>
     <sheet name="Login" sheetId="2" r:id="rId2"/>
     <sheet name="Create Acc" sheetId="3" r:id="rId3"/>
+    <sheet name="transfer" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>email</t>
   </si>
@@ -55,6 +56,51 @@
   </si>
   <si>
     <t>Displayname</t>
+  </si>
+  <si>
+    <t>pilihbank</t>
+  </si>
+  <si>
+    <t>destinationAC</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>swiftbank</t>
+  </si>
+  <si>
+    <t>benename</t>
+  </si>
+  <si>
+    <t>IBAN</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>world</t>
+  </si>
+  <si>
+    <t>ABCL76811692</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>BRIDJA0000</t>
+  </si>
+  <si>
+    <t>BRI</t>
+  </si>
+  <si>
+    <t>BNI</t>
+  </si>
+  <si>
+    <t>ajshjas</t>
   </si>
 </sst>
 </file>
@@ -62,10 +108,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -99,48 +145,47 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -154,18 +199,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -193,36 +231,44 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -249,37 +295,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -291,145 +463,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -458,37 +504,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -508,26 +543,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -555,158 +590,181 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1048,41 +1106,41 @@
   <sheetPr/>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="32.3333333333333" style="5" customWidth="1"/>
-    <col min="2" max="4" width="19.4444444444444" style="5" customWidth="1"/>
+    <col min="1" max="1" width="32.3333333333333" style="9" customWidth="1"/>
+    <col min="2" max="4" width="19.4444444444444" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="9" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1113,30 +1171,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="9" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1173,4 +1231,88 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="15.7777777777778" customWidth="1"/>
+    <col min="2" max="4" width="21.8888888888889" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.4444444444444" customWidth="1"/>
+    <col min="6" max="6" width="21.8888888888889" customWidth="1"/>
+    <col min="7" max="7" width="13.1111111111111" customWidth="1"/>
+    <col min="8" max="8" width="12.4444444444444" customWidth="1"/>
+    <col min="9" max="9" width="18.2222222222222" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="1">
+        <v>100</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>